<commit_message>
feat: normalization admin panel database and relatonal diagram
</commit_message>
<xml_diff>
--- a/adminpanel-normalization-db.xlsx
+++ b/adminpanel-normalization-db.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Documents\1 Ivan Workspace\02 Ivan\Projects\02 ivsm-ecommerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\OneDrive\Documentos\01 Ivan Workspace\02 Ivan\ivsm-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB38BB75-973F-4C88-98C0-C512E4E60C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52371097-0164-4040-82BD-D9681AA6ED57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="43">
   <si>
     <t>ADMIN PANEL DATABASE</t>
   </si>
@@ -49,13 +60,118 @@
   </si>
   <si>
     <t>name_permission</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>1FN</t>
+  </si>
+  <si>
+    <t>first_surname</t>
+  </si>
+  <si>
+    <t>second_surname</t>
+  </si>
+  <si>
+    <t>2FN</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ivans</t>
+  </si>
+  <si>
+    <t>Iván San Martín Santana</t>
+  </si>
+  <si>
+    <t>!KsjnJsueokñ1!"2</t>
+  </si>
+  <si>
+    <t>ivansanmartin987@gmail.com</t>
+  </si>
+  <si>
+    <t>Soporte Chat</t>
+  </si>
+  <si>
+    <t>client_attention</t>
+  </si>
+  <si>
+    <t>k!Ks83iebbvywpñ</t>
+  </si>
+  <si>
+    <t>Iván</t>
+  </si>
+  <si>
+    <t>San Martín</t>
+  </si>
+  <si>
+    <t>Santana</t>
+  </si>
+  <si>
+    <t>Esteban Kicks Trip</t>
+  </si>
+  <si>
+    <t>esteb</t>
+  </si>
+  <si>
+    <t>Esteban</t>
+  </si>
+  <si>
+    <t>Kicks</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>esteban.kicks2@gmail.com</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Staff_Permissions</t>
+  </si>
+  <si>
+    <t>staff_id</t>
+  </si>
+  <si>
+    <t>permission_id</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Staff_Roles</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Roles_Permissions</t>
+  </si>
+  <si>
+    <t>id_role</t>
+  </si>
+  <si>
+    <t>id_permission</t>
+  </si>
+  <si>
+    <t>3FN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +194,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +223,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,16 +286,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,51 +612,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:I10"/>
+  <dimension ref="B3:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="9">
+        <v>56976710201</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9">
+        <v>56931317421</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J12" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I10" s="2"/>
+      <c r="K12" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="9">
+        <v>56976710201</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="9">
+        <v>56931317421</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9">
+        <v>56976710201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="9">
+        <v>2</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="9">
+        <v>56931317421</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="9">
+        <v>56976710201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="9">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38" s="9">
+        <v>56931317421</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9">
+        <v>1</v>
+      </c>
+      <c r="D53" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{8618665D-6108-4FE9-A08E-ADB97AC17FF4}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{A8C0FE99-2E78-45E4-A29B-6CA71C890E21}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{D851721A-A234-4EAD-AF8E-3970294CA028}"/>
+    <hyperlink ref="H14" r:id="rId4" xr:uid="{ED51E5E5-7879-4C49-A320-37CE44D20427}"/>
+    <hyperlink ref="H20" r:id="rId5" xr:uid="{D04F6726-8D91-4AD2-826B-B28608487FC1}"/>
+    <hyperlink ref="H21" r:id="rId6" xr:uid="{D942955E-A644-445C-A39C-3EED47D6103E}"/>
+    <hyperlink ref="H37" r:id="rId7" xr:uid="{BC3BF9B1-07E6-44F1-AC0E-55AB0472BC39}"/>
+    <hyperlink ref="H38" r:id="rId8" xr:uid="{FD0CBC2C-5436-4C90-AF7E-715D1B1F845E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: admin panel and ecommerce relational model updated
</commit_message>
<xml_diff>
--- a/adminpanel-normalization-db.xlsx
+++ b/adminpanel-normalization-db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\OneDrive\Documentos\01 Ivan Workspace\02 Ivan\ivsm-ecommerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Documents\1 Ivan Workspace\02 Ivan\Projects\02 ivsm-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52371097-0164-4040-82BD-D9681AA6ED57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B29BA69-1CE6-42EF-AC8E-ABC1BB0DEC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="52">
   <si>
     <t>ADMIN PANEL DATABASE</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Soporte Chat</t>
   </si>
   <si>
-    <t>client_attention</t>
-  </si>
-  <si>
     <t>k!Ks83iebbvywpñ</t>
   </si>
   <si>
@@ -165,6 +162,36 @@
   </si>
   <si>
     <t>3FN</t>
+  </si>
+  <si>
+    <t>first_login</t>
+  </si>
+  <si>
+    <t>last_login</t>
+  </si>
+  <si>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>updated_by</t>
+  </si>
+  <si>
+    <t>created_by_staff</t>
+  </si>
+  <si>
+    <t>updated_by_staff</t>
+  </si>
+  <si>
+    <t>assigned_at</t>
+  </si>
+  <si>
+    <t>assigned_by_staff</t>
   </si>
 </sst>
 </file>
@@ -306,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -331,6 +358,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -612,33 +643,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K63"/>
+  <dimension ref="B3:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.77734375" customWidth="1"/>
     <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="17.21875" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:17" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -657,14 +695,32 @@
       <c r="G5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>1</v>
       </c>
@@ -683,45 +739,81 @@
       <c r="G6" s="9">
         <v>56976710201</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="17">
+        <v>45359</v>
+      </c>
+      <c r="I6" s="17">
+        <v>45359</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="17">
+        <v>45359</v>
+      </c>
+      <c r="M6" s="17">
+        <v>45359</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="9">
         <v>56931317421</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="17">
+        <v>45359</v>
+      </c>
+      <c r="I7" s="17">
+        <v>45359</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.3">
+      <c r="K7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="17">
+        <v>45359</v>
+      </c>
+      <c r="M7" s="17">
+        <v>45359</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="21" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>1</v>
       </c>
@@ -746,14 +838,32 @@
       <c r="I12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>1</v>
       </c>
@@ -761,13 +871,13 @@
         <v>14</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>16</v>
@@ -778,51 +888,87 @@
       <c r="I13" s="9">
         <v>56976710201</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K13" s="17">
+        <v>45359</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="17">
+        <v>45359</v>
+      </c>
+      <c r="O13" s="17">
+        <v>45359</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="I14" s="9">
         <v>56931317421</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K14" s="17">
+        <v>45359</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.3">
+      <c r="M14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="17">
+        <v>45359</v>
+      </c>
+      <c r="O14" s="17">
+        <v>45359</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="21" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
@@ -847,8 +993,14 @@
       <c r="I19" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>1</v>
       </c>
@@ -856,13 +1008,13 @@
         <v>14</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>16</v>
@@ -873,34 +1025,46 @@
       <c r="I20" s="9">
         <v>56976710201</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K20" s="17">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>2</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="I21" s="9">
         <v>56931317421</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K21" s="17">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>13</v>
       </c>
@@ -908,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
         <v>1</v>
       </c>
@@ -916,33 +1080,63 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="9">
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="17">
+        <v>45359</v>
+      </c>
+      <c r="E29" s="17">
+        <v>45359</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="32" spans="2:11" ht="21" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
@@ -967,8 +1161,14 @@
       <c r="I36" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="9">
         <v>1</v>
       </c>
@@ -976,13 +1176,13 @@
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>16</v>
@@ -993,66 +1193,78 @@
       <c r="I37" s="9">
         <v>56976710201</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K37" s="17">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="9">
         <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="G38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="I38" s="9">
         <v>56931317421</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J38" s="17">
+        <v>45359</v>
+      </c>
+      <c r="K38" s="17">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="9" t="s">
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="9">
-        <v>1</v>
-      </c>
-      <c r="D43" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" s="9">
         <v>1</v>
       </c>
@@ -1068,23 +1280,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="9">
         <v>1</v>
       </c>
@@ -1092,26 +1310,32 @@
         <v>1</v>
       </c>
       <c r="D53" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E53" s="17">
+        <v>45359</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="9">
         <v>1</v>
       </c>
@@ -1122,25 +1346,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="9">
         <v>1</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D63" s="17">
+        <v>45359</v>
+      </c>
+      <c r="E63" s="17">
+        <v>45359</v>
+      </c>
+      <c r="F63" s="9">
+        <v>1</v>
+      </c>
+      <c r="G63" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>